<commit_message>
Included Payer and Form in summary
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4BF8FC-A2A6-4CA4-9295-72FCA3BFB05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DFFBD8-2A8D-493B-9C16-79846913E3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -80,6 +80,9 @@
     <t>Form</t>
   </si>
   <si>
+    <t>Institutional (UB)</t>
+  </si>
+  <si>
     <t>Billing Provider</t>
   </si>
   <si>
@@ -122,7 +125,7 @@
     <t>End</t>
   </si>
   <si>
-    <t>Professional (CMS)</t>
+    <t>Payer</t>
   </si>
 </sst>
 </file>
@@ -293,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -324,6 +327,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,13 +342,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -659,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7759B226-B548-469F-A5B2-76DE4BBA961D}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -668,17 +668,17 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="26"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
@@ -688,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
@@ -711,127 +711,133 @@
     </row>
     <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="17"/>
-      <c r="B7" s="19"/>
-    </row>
-    <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A8" s="28" t="str">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="17"/>
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.6">
+      <c r="A9" s="27" t="str">
         <f>$B$2 &amp; " Only"</f>
-        <v>Professional (CMS) Only</v>
-      </c>
-      <c r="B8" s="29"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Rendering Provider", "Physician")</f>
-        <v>Rendering Provider</v>
-      </c>
-      <c r="B9" s="16"/>
+        <v>Institutional (UB) Only</v>
+      </c>
+      <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)","Facilities","Revenue Code")</f>
-        <v>Facilities</v>
+        <f>IF($B$2="Professional (CMS)", "Rendering Provider", "Physician")</f>
+        <v>Physician</v>
       </c>
       <c r="B10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)","Place of Service","Description")</f>
-        <v>Place of Service</v>
+        <f>IF($B$2="Professional (CMS)","Facilities","Revenue Code")</f>
+        <v>Revenue Code</v>
       </c>
       <c r="B11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "CPT Code", "CPT Code (SDC)")</f>
-        <v>CPT Code</v>
+        <f>IF($B$2="Professional (CMS)","Place of Service","Description")</f>
+        <v>Description</v>
       </c>
       <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Modifier", "CPT Code (Trans)")</f>
-        <v>Modifier</v>
+        <f>IF($B$2="Professional (CMS)", "CPT Code", "CPT Code (SDC)")</f>
+        <v>CPT Code (SDC)</v>
       </c>
       <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)","Diagnosis","Charges (SDC)")</f>
-        <v>Diagnosis</v>
+        <f>IF($B$2="Professional (CMS)", "Modifier", "CPT Code (Trans)")</f>
+        <v>CPT Code (Trans)</v>
       </c>
       <c r="B14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Charges", "Charges (Trans)")</f>
-        <v>Charges</v>
-      </c>
-      <c r="B15" s="25"/>
+        <f>IF($B$2="Professional (CMS)","Diagnosis","Charges (SDC)")</f>
+        <v>Charges (SDC)</v>
+      </c>
+      <c r="B15" s="20"/>
     </row>
     <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Units", "Units (SDC)")</f>
-        <v>Units</v>
-      </c>
-      <c r="B16" s="16"/>
+        <f>IF($B$2="Professional (CMS)", "Charges", "Charges (Trans)")</f>
+        <v>Charges (Trans)</v>
+      </c>
+      <c r="B16" s="20"/>
     </row>
     <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="str">
+        <f>IF($B$2="Professional (CMS)", "Units", "Units (SDC)")</f>
+        <v>Units (SDC)</v>
+      </c>
+      <c r="B17" s="16"/>
+    </row>
+    <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "", "Units (Trans)")</f>
-        <v/>
-      </c>
-      <c r="B17" s="16"/>
-    </row>
-    <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="17"/>
-      <c r="B18" s="19"/>
+        <v>Units (Trans)</v>
+      </c>
+      <c r="B18" s="16"/>
     </row>
     <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="24">
-        <f>COUNTA(Claims!A:A)-1</f>
-        <v>0</v>
-      </c>
+      <c r="A19" s="17"/>
+      <c r="B19" s="19"/>
     </row>
     <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="19">
+        <f>COUNTA(Claims!A:A)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="21">
         <f>SUM(Claims!E:E)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="21">
+    <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="22">
         <f>SUM(Claims!F:F)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="13"/>
-      <c r="B22" s="22"/>
+    <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="13"/>
+      <c r="B23" s="23"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Y/R11Z85Fd4+/EUPmKTn8lQNX+3q5nOd7xv0y/TaZuzc14OF5lvtZkDkfpAL3ki8H+hQl1okmRuRrWOsJrhUfQ==" saltValue="4wKzWEDl6NQwv7lF1S3qXA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="JxFbIcM+vpuOSyoUo+udb+kwc6MVYREhLTBr+zVB24/KAse0Rtnz4F6lqJbL+wC1z8atucrbGW4u77xxri+9dg==" saltValue="5OajXZajC7CChYk4KwHwjA==" spinCount="100000" sqref="A1:B1" name="Title"/>
   </protectedRanges>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
@@ -850,7 +856,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:L3"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,7 +887,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -893,17 +899,17 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="30"/>
+        <v>26</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="29"/>
       <c r="M1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +942,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F3"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -951,22 +957,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="9"/>

</xml_diff>

<commit_message>
Template info now in Excel
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DFFBD8-2A8D-493B-9C16-79846913E3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F85E25-A81A-42FC-B7C4-CFEBC2C4D701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Schedule</t>
   </si>
   <si>
-    <t>Insurance</t>
-  </si>
-  <si>
     <t>Claimbot Summary</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Form</t>
   </si>
   <si>
-    <t>Institutional (UB)</t>
-  </si>
-  <si>
     <t>Billing Provider</t>
   </si>
   <si>
@@ -125,7 +119,13 @@
     <t>End</t>
   </si>
   <si>
+    <t>Professional (CMS)</t>
+  </si>
+  <si>
     <t>Payer</t>
+  </si>
+  <si>
+    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -296,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -327,21 +327,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -668,32 +671,32 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" style="23" customWidth="1"/>
     <col min="3" max="3" width="3.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="27"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="16"/>
     </row>
@@ -705,19 +708,19 @@
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B7" s="16"/>
     </row>
@@ -726,72 +729,72 @@
       <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A9" s="27" t="str">
+      <c r="A9" s="28" t="str">
         <f>$B$2 &amp; " Only"</f>
-        <v>Institutional (UB) Only</v>
-      </c>
-      <c r="B9" s="28"/>
+        <v>Professional (CMS) Only</v>
+      </c>
+      <c r="B9" s="29"/>
     </row>
     <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "Rendering Provider", "Physician")</f>
-        <v>Physician</v>
+        <v>Rendering Provider</v>
       </c>
       <c r="B10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="str">
         <f>IF($B$2="Professional (CMS)","Facilities","Revenue Code")</f>
-        <v>Revenue Code</v>
+        <v>Facilities</v>
       </c>
       <c r="B11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="str">
         <f>IF($B$2="Professional (CMS)","Place of Service","Description")</f>
-        <v>Description</v>
+        <v>Place of Service</v>
       </c>
       <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "CPT Code", "CPT Code (SDC)")</f>
-        <v>CPT Code (SDC)</v>
+        <v>CPT Code</v>
       </c>
       <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "Modifier", "CPT Code (Trans)")</f>
-        <v>CPT Code (Trans)</v>
+        <v>Modifier</v>
       </c>
       <c r="B14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="str">
         <f>IF($B$2="Professional (CMS)","Diagnosis","Charges (SDC)")</f>
-        <v>Charges (SDC)</v>
-      </c>
-      <c r="B15" s="20"/>
+        <v>Diagnosis</v>
+      </c>
+      <c r="B15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "Charges", "Charges (Trans)")</f>
-        <v>Charges (Trans)</v>
-      </c>
-      <c r="B16" s="20"/>
+        <v>Charges</v>
+      </c>
+      <c r="B16" s="25"/>
     </row>
     <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "Units", "Units (SDC)")</f>
-        <v>Units (SDC)</v>
+        <v>Units</v>
       </c>
       <c r="B17" s="16"/>
     </row>
     <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "", "Units (Trans)")</f>
-        <v>Units (Trans)</v>
+        <v/>
       </c>
       <c r="B18" s="16"/>
     </row>
@@ -801,34 +804,34 @@
     </row>
     <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="19">
+        <v>21</v>
+      </c>
+      <c r="B20" s="24">
         <f>COUNTA(Claims!A:A)-1</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="21">
+        <v>22</v>
+      </c>
+      <c r="B21" s="20">
         <f>SUM(Claims!E:E)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="21">
         <f>SUM(Claims!F:F)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A23" s="13"/>
-      <c r="B23" s="23"/>
+      <c r="B23" s="22"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -856,7 +859,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -878,16 +881,16 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -899,17 +902,17 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="29"/>
+        <v>24</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="30"/>
       <c r="M1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +945,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,22 +960,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="9"/>

</xml_diff>

<commit_message>
Added bill type to summary
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F85E25-A81A-42FC-B7C4-CFEBC2C4D701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3DC57A-A32F-4FC9-9003-599CDA3065BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -119,13 +119,10 @@
     <t>End</t>
   </si>
   <si>
+    <t>Payer</t>
+  </si>
+  <si>
     <t>Professional (CMS)</t>
-  </si>
-  <si>
-    <t>Payer</t>
-  </si>
-  <si>
-    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -296,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -314,14 +311,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -342,7 +331,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -671,17 +672,17 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" style="21" customWidth="1"/>
     <col min="3" max="3" width="3.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
@@ -690,123 +691,124 @@
       <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>25</v>
+      <c r="B2" s="25" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="23"/>
     </row>
     <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="23"/>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="B5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="26"/>
     </row>
     <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
-    </row>
-    <row r="9" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A9" s="28" t="str">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.6">
+      <c r="A8" s="29" t="str">
         <f>$B$2 &amp; " Only"</f>
         <v>Professional (CMS) Only</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B8" s="30"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="str">
+        <f>IF($B$2="Professional (CMS)", "Rendering Provider", "Physician")</f>
+        <v>Rendering Provider</v>
+      </c>
+      <c r="B9" s="23"/>
     </row>
     <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Rendering Provider", "Physician")</f>
-        <v>Rendering Provider</v>
-      </c>
-      <c r="B10" s="16"/>
+        <f>IF($B$2="Professional (CMS)","Facilities","Bill Type")</f>
+        <v>Facilities</v>
+      </c>
+      <c r="B10" s="23"/>
     </row>
     <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)","Facilities","Revenue Code")</f>
-        <v>Facilities</v>
-      </c>
-      <c r="B11" s="16"/>
+        <f>IF($B$2="Professional (CMS)","Place of Service", "Revenue Code")</f>
+        <v>Place of Service</v>
+      </c>
+      <c r="B11" s="23"/>
     </row>
     <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)","Place of Service","Description")</f>
-        <v>Place of Service</v>
-      </c>
-      <c r="B12" s="16"/>
+        <f>IF($B$2="Professional (CMS)", "CPT Code", "Description")</f>
+        <v>CPT Code</v>
+      </c>
+      <c r="B12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "CPT Code", "CPT Code (SDC)")</f>
-        <v>CPT Code</v>
-      </c>
-      <c r="B13" s="16"/>
+        <f>IF($B$2="Professional (CMS)", "Modifier", "CPT Code (SDC)")</f>
+        <v>Modifier</v>
+      </c>
+      <c r="B13" s="23"/>
     </row>
     <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Modifier", "CPT Code (Trans)")</f>
-        <v>Modifier</v>
-      </c>
-      <c r="B14" s="16"/>
+        <f>IF($B$2="Professional (CMS)","Diagnosis","CPT Code (Trans)")</f>
+        <v>Diagnosis</v>
+      </c>
+      <c r="B14" s="23"/>
     </row>
     <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)","Diagnosis","Charges (SDC)")</f>
-        <v>Diagnosis</v>
-      </c>
-      <c r="B15" s="16"/>
+        <f>IF($B$2="Professional (CMS)", "Charges", "Charges (SDC)")</f>
+        <v>Charges</v>
+      </c>
+      <c r="B15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Charges", "Charges (Trans)")</f>
-        <v>Charges</v>
-      </c>
-      <c r="B16" s="25"/>
+        <f>IF($B$2="Professional (CMS)", "Units", "Charges (Trans)")</f>
+        <v>Units</v>
+      </c>
+      <c r="B16" s="23"/>
     </row>
     <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="str">
-        <f>IF($B$2="Professional (CMS)", "Units", "Units (SDC)")</f>
-        <v>Units</v>
-      </c>
-      <c r="B17" s="16"/>
+        <f>IF($B$2="Professional (CMS)", "", "Units (SDC)")</f>
+        <v/>
+      </c>
+      <c r="B17" s="23"/>
     </row>
     <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="str">
         <f>IF($B$2="Professional (CMS)", "", "Units (Trans)")</f>
         <v/>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="23"/>
     </row>
     <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="17"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="22">
         <f>COUNTA(Claims!A:A)-1</f>
         <v>0</v>
       </c>
@@ -815,23 +817,23 @@
       <c r="A21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="18">
         <f>SUM(Claims!E:E)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="19">
         <f>SUM(Claims!F:F)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A23" s="13"/>
-      <c r="B23" s="22"/>
+      <c r="B23" s="20"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -840,7 +842,7 @@
   </protectedRanges>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
@@ -907,10 +909,10 @@
       <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="30"/>
+      <c r="L1" s="31"/>
       <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
@@ -945,7 +947,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
If -1 total, claim submission failed conditional formatting
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3DC57A-A32F-4FC9-9003-599CDA3065BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D94C76C-A862-4AEF-B764-6A38486C50EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="166" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +159,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -175,13 +168,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,62 +287,59 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -367,7 +350,14 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -672,168 +662,168 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" style="18" customWidth="1"/>
     <col min="3" max="3" width="3.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="25"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="20"/>
     </row>
     <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="20"/>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="15"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A8" s="29" t="str">
+      <c r="A8" s="26" t="str">
         <f>$B$2 &amp; " Only"</f>
         <v>Professional (CMS) Only</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="str">
+      <c r="A9" s="11" t="str">
         <f>IF($B$2="Professional (CMS)", "Rendering Provider", "Physician")</f>
         <v>Rendering Provider</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="14" t="str">
+      <c r="A10" s="11" t="str">
         <f>IF($B$2="Professional (CMS)","Facilities","Bill Type")</f>
         <v>Facilities</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="20"/>
     </row>
     <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="14" t="str">
+      <c r="A11" s="11" t="str">
         <f>IF($B$2="Professional (CMS)","Place of Service", "Revenue Code")</f>
         <v>Place of Service</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="20"/>
     </row>
     <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="14" t="str">
+      <c r="A12" s="11" t="str">
         <f>IF($B$2="Professional (CMS)", "CPT Code", "Description")</f>
         <v>CPT Code</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="20"/>
     </row>
     <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="14" t="str">
+      <c r="A13" s="11" t="str">
         <f>IF($B$2="Professional (CMS)", "Modifier", "CPT Code (SDC)")</f>
         <v>Modifier</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="14" t="str">
+      <c r="A14" s="11" t="str">
         <f>IF($B$2="Professional (CMS)","Diagnosis","CPT Code (Trans)")</f>
         <v>Diagnosis</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="20"/>
     </row>
     <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="14" t="str">
+      <c r="A15" s="11" t="str">
         <f>IF($B$2="Professional (CMS)", "Charges", "Charges (SDC)")</f>
         <v>Charges</v>
       </c>
-      <c r="B15" s="24"/>
+      <c r="B15" s="21"/>
     </row>
     <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="14" t="str">
+      <c r="A16" s="11" t="str">
         <f>IF($B$2="Professional (CMS)", "Units", "Charges (Trans)")</f>
         <v>Units</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="20"/>
     </row>
     <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="14" t="str">
+      <c r="A17" s="11" t="str">
         <f>IF($B$2="Professional (CMS)", "", "Units (SDC)")</f>
         <v/>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="20"/>
     </row>
     <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="14" t="str">
+      <c r="A18" s="11" t="str">
         <f>IF($B$2="Professional (CMS)", "", "Units (Trans)")</f>
         <v/>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="20"/>
     </row>
     <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="15"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="19">
         <f>COUNTA(Claims!A:A)-1</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="18">
-        <f>SUM(Claims!E:E)</f>
+      <c r="B21" s="15">
+        <f>SUMIF(Claims!E:E, "&gt;0")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="16">
         <f>SUM(Claims!F:F)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="13"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -844,7 +834,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{79F520E3-04F1-40EA-8B2A-50EB9F67D5BB}">
       <formula1>"Professional (CMS), Institutional (UB)"</formula1>
@@ -861,7 +851,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:L3"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -869,8 +859,8 @@
     <col min="1" max="1" width="1.6328125" customWidth="1"/>
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
@@ -888,10 +878,10 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -909,10 +899,10 @@
       <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="31"/>
+      <c r="L1" s="28"/>
       <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
@@ -922,17 +912,17 @@
     <mergeCell ref="K1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>AND($J1&lt;TODAY(), $J1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:L1000">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="9">
       <formula>LEN(TRIM(K2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(M2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -943,11 +933,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28267B3C-E74E-4804-BB86-48CB16E884AA}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="A2:F3"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -956,11 +946,9 @@
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.6328125" customWidth="1"/>
     <col min="5" max="6" width="15.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -979,35 +967,26 @@
       <c r="F1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="H2" s="7">
-        <f>MONTH(D2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="G3" s="7">
-        <f>MONTH(C3)</f>
-        <v>1</v>
-      </c>
-      <c r="H3" s="7">
-        <f>MONTH(D3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C4" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Writes to excel after claim submission
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D94C76C-A862-4AEF-B764-6A38486C50EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BC9237-F091-46E9-BA6F-FB018067F4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -92,15 +92,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Claim Start</t>
-  </si>
-  <si>
-    <t>Claim End</t>
-  </si>
-  <si>
-    <t>Sent</t>
-  </si>
-  <si>
     <t>Paid</t>
   </si>
   <si>
@@ -123,6 +114,12 @@
   </si>
   <si>
     <t>Professional (CMS)</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
@@ -284,7 +281,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -330,6 +326,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,7 +659,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" style="17" customWidth="1"/>
     <col min="3" max="3" width="3.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6328125" customWidth="1"/>
@@ -673,45 +670,45 @@
         <v>4</v>
       </c>
       <c r="B1" s="25"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>26</v>
+      <c r="B2" s="21" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="20"/>
+      <c r="A5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="12"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="13"/>
     </row>
     <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.6">
       <c r="A8" s="26" t="str">
@@ -721,109 +718,109 @@
       <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)", "Rendering Provider", "Physician")</f>
+      <c r="A9" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)", "Rendering Provider", IF($B$2="Institutional (UB)", "Physician", "Error"))</f>
         <v>Rendering Provider</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)","Facilities","Bill Type")</f>
+      <c r="A10" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)","Facilities", IF($B$2="Institutional (UB)", "Bill Type", "Error"))</f>
         <v>Facilities</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)","Place of Service", "Revenue Code")</f>
+      <c r="A11" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)","Place of Service", IF($B$2="Institutional (UB)", "Revenue Code", "Error"))</f>
         <v>Place of Service</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)", "CPT Code", "Description")</f>
+      <c r="A12" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)", "CPT Code", IF($B$2="Institutional (UB)", "Description", "Error"))</f>
         <v>CPT Code</v>
       </c>
-      <c r="B12" s="20"/>
+      <c r="B12" s="19"/>
     </row>
     <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)", "Modifier", "CPT Code (SDC)")</f>
+      <c r="A13" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)", "Modifier", IF($B$2="Institutional (UB)", "CPT Code(SDC)", "Error"))</f>
         <v>Modifier</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)","Diagnosis","CPT Code (Trans)")</f>
+      <c r="A14" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)","Diagnosis",IF($B$2="Institutional (UB)", "CPT Code (Trans)", "Error"))</f>
         <v>Diagnosis</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)", "Charges", "Charges (SDC)")</f>
+      <c r="A15" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)", "Charges", IF($B$2="Institutional (UB)", "Charges (SDC)", "Error"))</f>
         <v>Charges</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="20"/>
     </row>
     <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)", "Units", "Charges (Trans)")</f>
+      <c r="A16" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)", "Units", IF($B$2="Institutional (UB)", "Charges (Trans)", "Error"))</f>
         <v>Units</v>
       </c>
-      <c r="B16" s="20"/>
+      <c r="B16" s="19"/>
     </row>
     <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)", "", "Units (SDC)")</f>
+      <c r="A17" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Units (SDC)", "Error"))</f>
         <v/>
       </c>
-      <c r="B17" s="20"/>
+      <c r="B17" s="19"/>
     </row>
     <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="11" t="str">
-        <f>IF($B$2="Professional (CMS)", "", "Units (Trans)")</f>
+      <c r="A18" s="10" t="str">
+        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Units (SDC)", "Error"))</f>
         <v/>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="19"/>
     </row>
     <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="12"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="13"/>
     </row>
     <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="19">
+      <c r="A20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="18">
         <f>COUNTA(Claims!A:A)-1</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="15">
-        <f>SUMIF(Claims!E:E, "&gt;0")</f>
+      <c r="A21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="14">
+        <f>SUMIF(Claims!D:D, "&gt;0")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="16">
-        <f>SUM(Claims!F:F)</f>
+      <c r="A22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="15">
+        <f>SUM(Claims!E:E)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -851,16 +848,16 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
@@ -878,10 +875,10 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -894,10 +891,10 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K1" s="28" t="s">
         <v>12</v>
@@ -933,22 +930,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28267B3C-E74E-4804-BB86-48CB16E884AA}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.6328125" customWidth="1"/>
-    <col min="5" max="6" width="15.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -956,33 +953,23 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C4" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="23"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
New summary value (description transportation)
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BC9237-F091-46E9-BA6F-FB018067F4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613D58FD-F687-4987-B083-A6B26F6C4527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -288,7 +288,6 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -301,9 +300,6 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -327,6 +323,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -659,168 +658,170 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" style="15" customWidth="1"/>
     <col min="3" max="3" width="3.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="24"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="20"/>
     </row>
     <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A8" s="26" t="str">
+      <c r="A8" s="25" t="str">
         <f>$B$2 &amp; " Only"</f>
         <v>Professional (CMS) Only</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="26"/>
     </row>
     <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="str">
+      <c r="A9" s="9" t="str">
         <f>IF($B$2="Professional (CMS)", "Rendering Provider", IF($B$2="Institutional (UB)", "Physician", "Error"))</f>
         <v>Rendering Provider</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="str">
+      <c r="A10" s="9" t="str">
         <f>IF($B$2="Professional (CMS)","Facilities", IF($B$2="Institutional (UB)", "Bill Type", "Error"))</f>
         <v>Facilities</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="str">
+      <c r="A11" s="9" t="str">
         <f>IF($B$2="Professional (CMS)","Place of Service", IF($B$2="Institutional (UB)", "Revenue Code", "Error"))</f>
         <v>Place of Service</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="17"/>
     </row>
     <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="str">
-        <f>IF($B$2="Professional (CMS)", "CPT Code", IF($B$2="Institutional (UB)", "Description", "Error"))</f>
+      <c r="A12" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)", "CPT Code", IF($B$2="Institutional (UB)", "Description (SDC)", "Error"))</f>
         <v>CPT Code</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="10" t="str">
-        <f>IF($B$2="Professional (CMS)", "Modifier", IF($B$2="Institutional (UB)", "CPT Code(SDC)", "Error"))</f>
+      <c r="A13" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)", "Modifier", IF($B$2="Institutional (UB)", "CPT Code (SDC)", "Error"))</f>
         <v>Modifier</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="17"/>
     </row>
     <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="10" t="str">
-        <f>IF($B$2="Professional (CMS)","Diagnosis",IF($B$2="Institutional (UB)", "CPT Code (Trans)", "Error"))</f>
+      <c r="A14" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)","Diagnosis",IF($B$2="Institutional (UB)", "Charges (SDC)", "Error"))</f>
         <v>Diagnosis</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="str">
-        <f>IF($B$2="Professional (CMS)", "Charges", IF($B$2="Institutional (UB)", "Charges (SDC)", "Error"))</f>
+      <c r="A15" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)", "Charges", IF($B$2="Institutional (UB)", "Units (SDC)", "Error"))</f>
         <v>Charges</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="18"/>
     </row>
     <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="10" t="str">
-        <f>IF($B$2="Professional (CMS)", "Units", IF($B$2="Institutional (UB)", "Charges (Trans)", "Error"))</f>
+      <c r="A16" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)", "Units", IF($B$2="Institutional (UB)", "Description (Trans)", "Error"))</f>
         <v>Units</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="17"/>
     </row>
     <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="str">
-        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Units (SDC)", "Error"))</f>
+      <c r="A17" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "CPT Code (Trans)", "Error"))</f>
         <v/>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="17"/>
     </row>
     <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="str">
-        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Units (SDC)", "Error"))</f>
+      <c r="A18" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Charges (Trans)", "Error"))</f>
         <v/>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="17"/>
     </row>
     <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="11"/>
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
+      <c r="A19" s="9" t="str">
+        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Units (Trans)", "Error"))</f>
+        <v/>
+      </c>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B21" s="16">
         <f>COUNTA(Claims!A:A)-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
+    <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B22" s="13">
         <f>SUMIF(Claims!D:D, "&gt;0")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="12" t="s">
+    <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B23" s="14">
         <f>SUM(Claims!E:E)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="9"/>
-      <c r="B23" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -848,7 +849,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -896,10 +897,10 @@
       <c r="J1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="28"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
@@ -930,11 +931,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28267B3C-E74E-4804-BB86-48CB16E884AA}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,10 +964,268 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="23"/>
+      <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="23"/>
+      <c r="A3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="21"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="21"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="21"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="21"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="21"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="21"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="21"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="21"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="21"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="21"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="21"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="21"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="21"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="21"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="21"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="21"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="21"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="21"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="21"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="21"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="21"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="21"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="21"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="21"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="21"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="21"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="21"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="21"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="21"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="21"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="21"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="21"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="21"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="21"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="21"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="21"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="21"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="21"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="21"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="21"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="21"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="21"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="21"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="21"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="21"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="21"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="21"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="21"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="21"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="21"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="21"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="21"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="21"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="21"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="21"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="21"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="21"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="21"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="21"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="21"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="21"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="21"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="21"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="21"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="21"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="21"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="21"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="21"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>

<commit_message>
Renamed summary to form
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AD756B-8572-42BB-A073-2B934E0F3556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B62B78-32C7-4F66-BA35-6B5FE72719A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="2" r:id="rId1"/>
+    <sheet name="Claim" sheetId="2" r:id="rId1"/>
     <sheet name="Insurance" sheetId="1" r:id="rId2"/>
-    <sheet name="Claims" sheetId="3" r:id="rId3"/>
+    <sheet name="Submitted" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">Claims!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Insurance!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">Submitted!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,9 +56,6 @@
     <t>Schedule</t>
   </si>
   <si>
-    <t>Claimbot Summary</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Range</t>
+  </si>
+  <si>
+    <t>Claimbot</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7759B226-B548-469F-A5B2-76DE4BBA961D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -663,7 +663,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
       <c r="A1" s="23" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B1" s="24"/>
       <c r="F1" s="8"/>
@@ -672,33 +672,33 @@
     </row>
     <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="20"/>
     </row>
@@ -795,28 +795,28 @@
     </row>
     <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="16">
-        <f>COUNTA(Claims!A:A)-1</f>
+        <f>COUNTA(Submitted!A:A)-1</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="13">
-        <f>SUMIF(Claims!D:D, "&gt;0")</f>
+        <f>SUMIF(Submitted!D:D, "&gt;0")</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="14">
-        <f>SUM(Claims!E:E)</f>
+        <f>SUM(Submitted!E:E)</f>
         <v>0</v>
       </c>
     </row>
@@ -844,7 +844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -867,13 +867,13 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -885,17 +885,17 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="J1" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="27"/>
       <c r="L1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -941,19 +941,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added IDs for members
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B62B78-32C7-4F66-BA35-6B5FE72719A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9784062-EFE8-4696-8F74-8D977B6F8050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Claimbot</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -842,11 +845,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -865,7 +868,10 @@
     <col min="12" max="12" width="7.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updated protection of templates
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMERICAN SENIOR CARE\Desktop\claimbot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D85DFF-5364-4E7C-8B2B-FC49B3CC22F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53CB826-A044-4EB3-87D3-AA3B52A45788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5610" yWindow="4215" windowWidth="15510" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Claim" sheetId="2" r:id="rId1"/>
@@ -318,24 +318,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -352,6 +337,21 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -663,28 +663,28 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="3.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.6328125" customWidth="1"/>
+    <col min="5" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="25"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -692,122 +692,122 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="13"/>
     </row>
-    <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A8" s="17" t="str">
+    <row r="8" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="26" t="str">
         <f>$B$2 &amp; " Only"</f>
         <v>Professional (CMS) Only</v>
       </c>
-      <c r="B8" s="18"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "Rendering Provider", IF($B$2="Institutional (UB)", "Physician", "Error"))</f>
         <v>Rendering Provider</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="str">
         <f>IF($B$2="Professional (CMS)","Facilities", IF($B$2="Institutional (UB)", "Bill Type", "Error"))</f>
         <v>Facilities</v>
       </c>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="str">
         <f>IF($B$2="Professional (CMS)","Place of Service", IF($B$2="Institutional (UB)", "Revenue Code", "Error"))</f>
         <v>Place of Service</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "CPT Code", IF($B$2="Institutional (UB)", "Description (SDC)", "Error"))</f>
         <v>CPT Code</v>
       </c>
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "Modifier", IF($B$2="Institutional (UB)", "CPT Code (SDC)", "Error"))</f>
         <v>Modifier</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="str">
         <f>IF($B$2="Professional (CMS)","Diagnosis",IF($B$2="Institutional (UB)", "Charges (SDC)", "Error"))</f>
         <v>Diagnosis</v>
       </c>
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "Charges", IF($B$2="Institutional (UB)", "Units (SDC)", "Error"))</f>
         <v>Charges</v>
       </c>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "Units", IF($B$2="Institutional (UB)", "Description (Trans)", "Error"))</f>
         <v>Units</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "CPT Code (Trans)", "Error"))</f>
         <v/>
       </c>
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Charges (Trans)", "Error"))</f>
         <v/>
       </c>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="13"/>
+    </row>
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="str">
         <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Units (Trans)", "Error"))</f>
         <v/>
       </c>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
     </row>
-    <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
@@ -835,7 +835,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="JxFbIcM+vpuOSyoUo+udb+kwc6MVYREhLTBr+zVB24/KAse0Rtnz4F6lqJbL+wC1z8atucrbGW4u77xxri+9dg==" saltValue="5OajXZajC7CChYk4KwHwjA==" spinCount="100000" sqref="A1:B1" name="Title"/>
   </protectedRanges>
@@ -860,64 +860,64 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.453125" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.453125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.453125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.1796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="23"/>
+    <col min="1" max="1" width="3.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="21" t="s">
+      <c r="K1" s="28"/>
+      <c r="L1" s="17" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
@@ -943,304 +943,302 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28267B3C-E74E-4804-BB86-48CB16E884AA}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="23"/>
+    <col min="1" max="1" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="26"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="26"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="26"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="26"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="26"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="26"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="26"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="26"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="26"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="26"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="26"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="26"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="26"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="26"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="26"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="26"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="26"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="26"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="26"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="26"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="26"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="26"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="26"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="26"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="26"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="26"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="26"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="26"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="26"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="26"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="26"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="26"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="26"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="26"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="26"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="26"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="26"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="26"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="26"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="26"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="26"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="26"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="26"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="26"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="26"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" s="26"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="26"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" s="26"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="26"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="26"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="26"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="26"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="26"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="26"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="26"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="26"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="26"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" s="26"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" s="26"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="26"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="26"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="26"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="26"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" s="26"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" s="26"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="26"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" s="26"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" s="26"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84" s="26"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="26"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" s="26"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" s="26"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88" s="26"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" s="26"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="21"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="21"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="21"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="21"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="21"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="21"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>

</xml_diff>

<commit_message>
Allowed CMS template to have second set of cpt
</commit_message>
<xml_diff>
--- a/assets/Blank Template.xlsx
+++ b/assets/Blank Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMERICAN SENIOR CARE\Desktop\claimbot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53CB826-A044-4EB3-87D3-AA3B52A45788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D902DFC2-AAD0-4210-B46B-C15646CBB2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="4215" windowWidth="15510" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="3930" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Claim" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -56,6 +56,21 @@
     <t>Schedule</t>
   </si>
   <si>
+    <t>ABC123123123</t>
+  </si>
+  <si>
+    <t>M15.0</t>
+  </si>
+  <si>
+    <t>1.2.3.4.5</t>
+  </si>
+  <si>
+    <t>XYZ321321321</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
     <t>Username</t>
   </si>
   <si>
@@ -71,6 +86,18 @@
     <t>Birth Date</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>McGee</t>
+  </si>
+  <si>
     <t>Form</t>
   </si>
   <si>
@@ -120,6 +147,15 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>CPT Code (2)</t>
+  </si>
+  <si>
+    <t>Charges (2)</t>
+  </si>
+  <si>
+    <t>Units (2)</t>
   </si>
 </sst>
 </file>
@@ -318,18 +354,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -677,7 +713,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="24" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B1" s="25"/>
       <c r="F1" s="1"/>
@@ -686,33 +722,33 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B6" s="13"/>
     </row>
@@ -750,57 +786,54 @@
     </row>
     <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)", "CPT Code", IF($B$2="Institutional (UB)", "Description (SDC)", "Error"))</f>
-        <v>CPT Code</v>
+        <f>IF($B$2="Professional (CMS)", "Modifier", IF($B$2="Institutional (UB)", "Description (1)", "Error"))</f>
+        <v>Modifier</v>
       </c>
       <c r="B12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)", "Modifier", IF($B$2="Institutional (UB)", "CPT Code (SDC)", "Error"))</f>
-        <v>Modifier</v>
+        <f>IF($B$2="Professional (CMS)", "Diagnosis", IF($B$2="Institutional (UB)", "CPT Code (1)", "Error"))</f>
+        <v>Diagnosis</v>
       </c>
       <c r="B13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)","Diagnosis",IF($B$2="Institutional (UB)", "Charges (SDC)", "Error"))</f>
-        <v>Diagnosis</v>
+        <f>IF($B$2="Professional (CMS)","CPT Code (1)",IF($B$2="Institutional (UB)", "Charges (1)", "Error"))</f>
+        <v>CPT Code (1)</v>
       </c>
       <c r="B14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)", "Charges", IF($B$2="Institutional (UB)", "Units (SDC)", "Error"))</f>
-        <v>Charges</v>
+        <f>IF($B$2="Professional (CMS)", "Charges (1)", IF($B$2="Institutional (UB)", "Units (1)", "Error"))</f>
+        <v>Charges (1)</v>
       </c>
       <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)", "Units", IF($B$2="Institutional (UB)", "Description (Trans)", "Error"))</f>
-        <v>Units</v>
+        <f>IF($B$2="Professional (CMS)", "Units (1)", IF($B$2="Institutional (UB)", "Description (2)", "Error"))</f>
+        <v>Units (1)</v>
       </c>
       <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "CPT Code (Trans)", "Error"))</f>
-        <v/>
+      <c r="A17" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B17" s="10"/>
     </row>
     <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Charges (Trans)", "Error"))</f>
-        <v/>
-      </c>
-      <c r="B18" s="13"/>
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="10"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="str">
-        <f>IF($B$2="Professional (CMS)", "", IF($B$2="Institutional (UB)", "Units (Trans)", "Error"))</f>
-        <v/>
+      <c r="A19" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B19" s="13"/>
     </row>
@@ -809,7 +842,7 @@
     </row>
     <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B21" s="9">
         <f>COUNTA(Submitted!A:A)-1</f>
@@ -818,7 +851,7 @@
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B22" s="6">
         <f>SUMIF(Submitted!D:D, "&gt;0")</f>
@@ -827,7 +860,7 @@
     </row>
     <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B23" s="7">
         <f>SUM(Submitted!E:E)</f>
@@ -856,64 +889,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="18"/>
+    <col min="1" max="1" width="3.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="28"/>
+      <c r="L1" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="16">
+        <v>20791</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="H2" s="17">
+        <v>45383</v>
+      </c>
+      <c r="I2" s="17">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="16">
+        <v>17699</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="17" t="s">
-        <v>12</v>
+      <c r="H3" s="17">
+        <v>45383</v>
+      </c>
+      <c r="I3" s="17">
+        <v>45731</v>
+      </c>
+      <c r="J3" s="17">
+        <v>45417</v>
+      </c>
+      <c r="K3" s="17">
+        <v>45422</v>
       </c>
     </row>
   </sheetData>
@@ -943,37 +1040,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28267B3C-E74E-4804-BB86-48CB16E884AA}">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="18"/>
+    <col min="6" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1236,6 +1333,9 @@
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="21"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="21"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>